<commit_message>
add document for screenshots
</commit_message>
<xml_diff>
--- a/Document/Work_Estimate_PROSOUL.xlsx
+++ b/Document/Work_Estimate_PROSOUL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anuradha\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prosoul_projects\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB98175A-660C-4AF0-97C6-B625DF6F72E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C919ABE-3ACA-4454-B168-01E5CAD4B090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{5F0C9D4C-AB25-493F-9A09-BE5A7B5A1A8A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>MASTER</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>PENDING</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,10 +188,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +507,7 @@
   <dimension ref="A2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +541,7 @@
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -549,7 +552,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
@@ -558,11 +561,11 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -572,9 +575,9 @@
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="7"/>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -584,9 +587,9 @@
       <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="7"/>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -596,10 +599,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
@@ -616,15 +619,15 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H8" t="s">
@@ -632,160 +635,160 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="5"/>
       <c r="H9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="5"/>
       <c r="H10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="5"/>
       <c r="H11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="5"/>
       <c r="H12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="5">
         <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="6"/>
       <c r="F15" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="5"/>
       <c r="H15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="6"/>
       <c r="F16" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="5"/>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="6"/>
       <c r="F17" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="5"/>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="6"/>
       <c r="F18" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="5"/>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="6"/>
       <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="5"/>
       <c r="H19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -793,13 +796,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G8:G12"/>
     <mergeCell ref="B7:B13"/>
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="G14:G19"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G8:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>